<commit_message>
new features of alphabetical sort, input focus, and tag suggestions
</commit_message>
<xml_diff>
--- a/server/Data.xlsx
+++ b/server/Data.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -417,16 +417,67 @@
       <c r="C2" t="str">
         <v>2</v>
       </c>
+      <c r="D2" t="str">
+        <v>a</v>
+      </c>
+      <c r="E2" t="str">
+        <v>c</v>
+      </c>
+      <c r="F2" t="str">
+        <v>b</v>
+      </c>
+      <c r="G2" t="str">
+        <v>x</v>
+      </c>
+      <c r="H2" t="str">
+        <v>e</v>
+      </c>
+      <c r="I2" t="str">
+        <v>f</v>
+      </c>
+      <c r="J2" t="str">
+        <v>g</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
         <v>c</v>
       </c>
+      <c r="B3" t="str">
+        <v>new</v>
+      </c>
+      <c r="C3" t="str">
+        <v>hi</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
         <v>d</v>
       </c>
+      <c r="B4" t="str">
+        <v>hello</v>
+      </c>
+      <c r="C4" t="str">
+        <v>hi</v>
+      </c>
+      <c r="D4" t="str">
+        <v>new</v>
+      </c>
+      <c r="E4" t="str">
+        <v>hey</v>
+      </c>
+      <c r="F4" t="str">
+        <v>help</v>
+      </c>
+      <c r="G4" t="str">
+        <v>heyow</v>
+      </c>
+      <c r="H4" t="str">
+        <v>helpo</v>
+      </c>
+      <c r="I4" t="str">
+        <v>helpo</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
@@ -438,6 +489,12 @@
       <c r="C5" t="str">
         <v>9</v>
       </c>
+      <c r="D5" t="str">
+        <v>new tag</v>
+      </c>
+      <c r="E5" t="str">
+        <v>banana</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
@@ -446,7 +503,7 @@
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:J6"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>